<commit_message>
update login và order thiết kế
</commit_message>
<xml_diff>
--- a/Bao_cao/Thiết kế/Thiết kế chi tiết/MILKTEAMANAGEMENT_TLPT_01_LogIn.xlsx
+++ b/Bao_cao/Thiết kế/Thiết kế chi tiết/MILKTEAMANAGEMENT_TLPT_01_LogIn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210" tabRatio="826" activeTab="1"/>
+    <workbookView windowWidth="22188" windowHeight="9024" tabRatio="826" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_bìa" sheetId="19" r:id="rId1"/>
@@ -538,10 +538,10 @@
     <t>Truy xuất</t>
   </si>
   <si>
-    <t>username</t>
+    <t>User.object.get().username</t>
   </si>
   <si>
-    <t>password</t>
+    <t>User.object.get().password</t>
   </si>
   <si>
     <t>user_id</t>
@@ -3863,8 +3863,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3762375" y="23780750"/>
-          <a:ext cx="746125" cy="971550"/>
+          <a:off x="3396615" y="23780750"/>
+          <a:ext cx="664845" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3928,8 +3928,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3616325" y="25333325"/>
-          <a:ext cx="1044575" cy="647700"/>
+          <a:off x="3270885" y="25333325"/>
+          <a:ext cx="935355" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="can">
           <a:avLst>
@@ -3987,7 +3987,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4135120" y="24752300"/>
+          <a:off x="3728720" y="24752300"/>
           <a:ext cx="5080" cy="581025"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -4044,8 +4044,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2571750" y="23533100"/>
-          <a:ext cx="3038475" cy="2609850"/>
+          <a:off x="2327910" y="23533100"/>
+          <a:ext cx="2733675" cy="2609850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4103,8 +4103,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3441700" y="23256875"/>
-          <a:ext cx="1308100" cy="428625"/>
+          <a:off x="3108960" y="23256875"/>
+          <a:ext cx="1173480" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4172,8 +4172,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="406400" y="24209375"/>
-          <a:ext cx="1082675" cy="400050"/>
+          <a:off x="365760" y="24209375"/>
+          <a:ext cx="981075" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4282,8 +4282,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1593850" y="24342725"/>
-          <a:ext cx="2073275" cy="0"/>
+          <a:off x="1451610" y="24342725"/>
+          <a:ext cx="1849755" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4339,8 +4339,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4787900" y="24304625"/>
-          <a:ext cx="2070100" cy="0"/>
+          <a:off x="4320540" y="24304625"/>
+          <a:ext cx="1866900" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4396,8 +4396,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6918325" y="24647525"/>
-          <a:ext cx="984250" cy="400050"/>
+          <a:off x="6227445" y="24647525"/>
+          <a:ext cx="902970" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4495,8 +4495,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7061200" y="23780750"/>
-          <a:ext cx="746125" cy="971550"/>
+          <a:off x="6370320" y="23780750"/>
+          <a:ext cx="664845" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4560,8 +4560,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6899275" y="26209625"/>
-          <a:ext cx="984250" cy="400050"/>
+          <a:off x="6217920" y="26209625"/>
+          <a:ext cx="893445" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4726,8 +4726,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7042150" y="25342850"/>
-          <a:ext cx="746125" cy="971550"/>
+          <a:off x="6351270" y="25342850"/>
+          <a:ext cx="664845" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4791,8 +4791,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="2640000">
-          <a:off x="4408805" y="25453340"/>
-          <a:ext cx="2679700" cy="35560"/>
+          <a:off x="3982085" y="25453340"/>
+          <a:ext cx="2415540" cy="35560"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4851,8 +4851,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1943100" y="2047875"/>
-          <a:ext cx="5264150" cy="419100"/>
+          <a:off x="1760220" y="2044065"/>
+          <a:ext cx="4735830" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4917,8 +4917,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="393700" y="2076450"/>
-          <a:ext cx="8379460" cy="4154805"/>
+          <a:off x="365760" y="2072640"/>
+          <a:ext cx="7533640" cy="4154805"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4954,8 +4954,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2108200" y="1066800"/>
-          <a:ext cx="5949950" cy="5467350"/>
+          <a:off x="1905000" y="1059180"/>
+          <a:ext cx="5360670" cy="5345430"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5022,7 +5022,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5097,7 +5097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5172,7 +5172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5247,7 +5247,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5322,7 +5322,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5397,7 +5397,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5472,7 +5472,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5547,7 +5547,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5622,7 +5622,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5697,7 +5697,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5772,7 +5772,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5847,7 +5847,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5922,7 +5922,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5997,7 +5997,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6072,7 +6072,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6147,7 +6147,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6222,7 +6222,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6297,7 +6297,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6372,7 +6372,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6447,7 +6447,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6522,7 +6522,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6597,7 +6597,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6672,7 +6672,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6747,7 +6747,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6822,7 +6822,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6897,7 +6897,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6972,7 +6972,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7047,7 +7047,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7122,7 +7122,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7197,7 +7197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7272,7 +7272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7347,7 +7347,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7422,7 +7422,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7497,7 +7497,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7572,7 +7572,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7647,7 +7647,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7722,7 +7722,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7797,7 +7797,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7872,7 +7872,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7947,7 +7947,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8022,7 +8022,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8097,7 +8097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8172,7 +8172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8247,7 +8247,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8322,7 +8322,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8397,7 +8397,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8472,7 +8472,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8547,7 +8547,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8622,7 +8622,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8697,7 +8697,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8772,7 +8772,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8847,7 +8847,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8922,7 +8922,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8997,7 +8997,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9072,7 +9072,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9147,7 +9147,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9222,7 +9222,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9297,7 +9297,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9372,7 +9372,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9447,7 +9447,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9522,7 +9522,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9597,7 +9597,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9672,7 +9672,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9747,7 +9747,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9822,7 +9822,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9897,7 +9897,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9972,7 +9972,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10047,7 +10047,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10122,7 +10122,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10197,7 +10197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10272,7 +10272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10347,7 +10347,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10422,7 +10422,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10497,7 +10497,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10572,7 +10572,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10647,7 +10647,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10722,7 +10722,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10797,7 +10797,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10872,7 +10872,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10947,7 +10947,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11022,7 +11022,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11097,7 +11097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11172,7 +11172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11247,7 +11247,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11322,7 +11322,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11397,7 +11397,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11472,7 +11472,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11547,7 +11547,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11622,7 +11622,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11697,7 +11697,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11772,7 +11772,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11847,7 +11847,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11922,7 +11922,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11997,7 +11997,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12072,7 +12072,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12147,7 +12147,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12222,7 +12222,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12297,7 +12297,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12372,7 +12372,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12447,7 +12447,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12522,7 +12522,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12597,7 +12597,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12672,7 +12672,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12747,7 +12747,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12822,7 +12822,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12897,7 +12897,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12972,7 +12972,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13047,7 +13047,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13122,7 +13122,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13197,7 +13197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13272,7 +13272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13347,7 +13347,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13422,7 +13422,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13497,7 +13497,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13572,7 +13572,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13647,7 +13647,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13722,7 +13722,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13797,7 +13797,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13872,7 +13872,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13947,7 +13947,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14022,7 +14022,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14097,7 +14097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14172,7 +14172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14247,7 +14247,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14322,7 +14322,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14397,7 +14397,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14472,7 +14472,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14547,7 +14547,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14622,7 +14622,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14697,7 +14697,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14772,7 +14772,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14847,7 +14847,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14922,7 +14922,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14997,7 +14997,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15072,7 +15072,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15147,7 +15147,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15222,7 +15222,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15297,7 +15297,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15372,7 +15372,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15447,7 +15447,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15522,7 +15522,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15597,7 +15597,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15672,7 +15672,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3889375" y="0"/>
+          <a:off x="3503295" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15747,7 +15747,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15822,7 +15822,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15897,7 +15897,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15972,7 +15972,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16047,7 +16047,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16122,7 +16122,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16197,7 +16197,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16272,7 +16272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16347,7 +16347,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4295775" y="0"/>
+          <a:off x="3869055" y="0"/>
           <a:ext cx="47625" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -16422,8 +16422,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5232400" y="1409700"/>
-          <a:ext cx="2159000" cy="962025"/>
+          <a:off x="4724400" y="1394460"/>
+          <a:ext cx="1935480" cy="942975"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -16488,8 +16488,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1914525" y="1504950"/>
-          <a:ext cx="552450" cy="428625"/>
+          <a:off x="1731645" y="1489710"/>
+          <a:ext cx="491490" cy="417195"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -16532,8 +16532,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6073775" y="2609850"/>
-          <a:ext cx="438150" cy="1590675"/>
+          <a:off x="5484495" y="2567940"/>
+          <a:ext cx="377190" cy="1556385"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -16576,8 +16576,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2609850" y="4324350"/>
-          <a:ext cx="4838700" cy="533400"/>
+          <a:off x="2366010" y="4244340"/>
+          <a:ext cx="4351020" cy="521970"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -16642,8 +16642,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6172200" y="5029200"/>
-          <a:ext cx="434975" cy="552450"/>
+          <a:off x="5562600" y="4933950"/>
+          <a:ext cx="394335" cy="541020"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -16686,8 +16686,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5232400" y="5695950"/>
-          <a:ext cx="2263775" cy="561975"/>
+          <a:off x="4724400" y="5585460"/>
+          <a:ext cx="2040255" cy="550545"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -16752,8 +16752,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2628900" y="3076575"/>
-          <a:ext cx="2159000" cy="514350"/>
+          <a:off x="2377440" y="3027045"/>
+          <a:ext cx="1943100" cy="502920"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -16818,8 +16818,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2590800" y="1409700"/>
-          <a:ext cx="2159000" cy="981075"/>
+          <a:off x="2346960" y="1394460"/>
+          <a:ext cx="1935480" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -16884,8 +16884,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3441700" y="2581275"/>
-          <a:ext cx="438150" cy="400050"/>
+          <a:off x="3108960" y="2539365"/>
+          <a:ext cx="384810" cy="392430"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -16928,8 +16928,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3441700" y="3686175"/>
-          <a:ext cx="438150" cy="542925"/>
+          <a:off x="3108960" y="3621405"/>
+          <a:ext cx="384810" cy="531495"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst>
@@ -16972,8 +16972,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="346075" y="1066800"/>
-          <a:ext cx="1441450" cy="1333500"/>
+          <a:off x="325755" y="1059180"/>
+          <a:ext cx="1299210" cy="1306830"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17033,8 +17033,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7642225" y="2590800"/>
-          <a:ext cx="1762125" cy="2143125"/>
+          <a:off x="6890385" y="2548890"/>
+          <a:ext cx="1579245" cy="2097405"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -17170,8 +17170,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8280400" y="1066800"/>
-          <a:ext cx="1327150" cy="1295400"/>
+          <a:off x="7467600" y="1059180"/>
+          <a:ext cx="1184910" cy="1268730"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17231,8 +17231,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7594600" y="1485900"/>
-          <a:ext cx="552450" cy="428625"/>
+          <a:off x="6842760" y="1470660"/>
+          <a:ext cx="491490" cy="417195"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -17277,8 +17277,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10099675" y="200025"/>
-          <a:ext cx="987425" cy="533400"/>
+          <a:off x="9103995" y="200025"/>
+          <a:ext cx="885825" cy="529590"/>
         </a:xfrm>
         <a:prstGeom prst="bevel">
           <a:avLst>
@@ -17347,7 +17347,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="114300" y="76200"/>
-              <a:ext cx="1612900" cy="260350"/>
+              <a:ext cx="1450340" cy="260350"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -26471,8 +26471,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:BJ180"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="AJ169" sqref="AJ169"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="AA157" sqref="AA157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="13.5" customHeight="1"/>
@@ -26718,7 +26718,7 @@
       <c r="AV4" s="165"/>
       <c r="AW4" s="185"/>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" ht="13.2" spans="1:49">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>62</v>
@@ -36369,9 +36369,9 @@
       <selection activeCell="A1" sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="13.2"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:49">
+    <row r="1" s="1" customFormat="1" ht="13.5" customHeight="1" spans="1:49">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -36438,7 +36438,7 @@
       <c r="AV1" s="38"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:49">
+    <row r="2" s="1" customFormat="1" ht="13.5" customHeight="1" spans="1:49">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -36601,7 +36601,7 @@
       <c r="AV4" s="10"/>
       <c r="AW4" s="47"/>
     </row>
-    <row r="5" s="2" customFormat="1" customHeight="1" spans="1:49">
+    <row r="5" s="2" customFormat="1" ht="13.5" customHeight="1" spans="1:49">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -38480,7 +38480,7 @@
       <c r="AV41" s="10"/>
       <c r="AW41" s="47"/>
     </row>
-    <row r="42" s="2" customFormat="1" customHeight="1" spans="1:49">
+    <row r="42" s="2" customFormat="1" ht="13.5" customHeight="1" spans="1:49">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>

</xml_diff>